<commit_message>
IO excel write for shopTest fix
</commit_message>
<xml_diff>
--- a/shopDataTest.xlsx
+++ b/shopDataTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QAC\IdeaProjects\selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BE52AF-6321-4493-9D93-A1C828ED139B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC873BE-A1AC-4899-BB1B-228FD20BA2FA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9960" windowHeight="8850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,12 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
-    <t xml:space="preserve">email </t>
-  </si>
-  <si>
-    <t>test@user.com</t>
-  </si>
-  <si>
     <t>First name</t>
   </si>
   <si>
@@ -58,9 +52,6 @@
     <t>forever</t>
   </si>
   <si>
-    <t xml:space="preserve">City </t>
-  </si>
-  <si>
     <t>Wakanda</t>
   </si>
   <si>
@@ -71,16 +62,33 @@
   </si>
   <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>abc155553@test.com</t>
+  </si>
+  <si>
+    <t>City</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -103,13 +111,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,42 +436,42 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>555555888</v>
@@ -468,7 +479,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>8888</v>
@@ -476,42 +487,45 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{E937399A-BCBC-40FC-A715-1766F6F9C180}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>